<commit_message>
Planningen en foto's ontwerpen
</commit_message>
<xml_diff>
--- a/Teamkalender.xlsx
+++ b/Teamkalender.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03BC7157-35DB-49AE-A237-D2384A0794D0}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be8eab015e44bd96/Documenten/P^0O 2/GIT/2022_2023_Probleemoplossen_en_Ontwerpen_2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="161" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62F82A66-953A-4F8F-A765-23BDB615D7A0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -66,9 +69,6 @@
     <t>indienen plannningen</t>
   </si>
   <si>
-    <t>theorielessen over applicaties</t>
-  </si>
-  <si>
     <t>27/02-05/03</t>
   </si>
   <si>
@@ -135,32 +135,20 @@
     <t>22/05-28/05</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">indienen verslag </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>deadline: verslag schrijven en powerpoint</t>
-    </r>
-  </si>
-  <si>
     <t>Presentatie</t>
+  </si>
+  <si>
+    <t>indienen verslag + ppt</t>
+  </si>
+  <si>
+    <t>theorielessen applicaties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,11 +175,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -251,7 +234,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -267,7 +250,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -565,17 +548,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="9" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="9" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -604,7 +587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1">
+    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -612,7 +595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30.75" customHeight="1">
+    <row r="4" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -623,146 +606,146 @@
         <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="30.75" customHeight="1">
+    <row r="6" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30.75" customHeight="1">
+    <row r="7" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="5" t="s">
+    </row>
+    <row r="10" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="30.75" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
         <v>24</v>
       </c>
-      <c r="I12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30.75" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>31</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>